<commit_message>
2.7 General bug fixes. Functioning drone logic.
</commit_message>
<xml_diff>
--- a/Drone Manual.xlsx
+++ b/Drone Manual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoel1\Documents\Yoel\FIU\APAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55FC6D0-1D82-4738-99C2-BB138634FCA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57664B10-12ED-432D-AC5E-B69D4CB65052}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DD67ECB3-E821-4B91-81DE-64EE5DC6E604}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="87">
   <si>
     <t>Drone GUI</t>
   </si>
@@ -284,6 +284,18 @@
   </si>
   <si>
     <t>Note: yellow IDs won't be used in protcol</t>
+  </si>
+  <si>
+    <t>Fly</t>
+  </si>
+  <si>
+    <t>Drone is flying</t>
+  </si>
+  <si>
+    <t>Flying Mode</t>
+  </si>
+  <si>
+    <t>Flying Mode when in flying</t>
   </si>
 </sst>
 </file>
@@ -320,7 +332,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -343,8 +355,14 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -435,6 +453,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -442,7 +504,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -456,6 +518,18 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -481,7 +555,7 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -500,6 +574,13 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -720,16 +801,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>151111</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>189211</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>83824</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>141326</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>369574</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>179426</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -752,7 +833,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9086850" y="913111"/>
+          <a:off x="8753475" y="570211"/>
           <a:ext cx="6770374" cy="5514715"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -771,7 +852,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{6808A5A3-C3E6-4B4D-B1D3-DCD3D9383298}" name="Button"/>
     <tableColumn id="2" xr3:uid="{1949676E-B3CF-47EA-B18C-6D1900FC5AB8}" name="Description"/>
-    <tableColumn id="3" xr3:uid="{89D6C74B-2760-4C5F-8F18-1E8C087BAAF0}" name="int ID" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{89D6C74B-2760-4C5F-8F18-1E8C087BAAF0}" name="int ID" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -781,8 +862,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{12DFBBD7-37B7-454B-871A-7C28D3202544}" name="Table3" displayName="Table3" ref="B10:D19" totalsRowShown="0">
   <autoFilter ref="B10:D19" xr:uid="{95C09762-773D-48C7-8580-A10D282A8995}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1D14631D-3961-4AEE-A677-8C5EF13E836C}" name="Status" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{6CEE09D4-5D6F-4E0A-9BE9-AE0EC38CA0B1}" name="Name" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{1D14631D-3961-4AEE-A677-8C5EF13E836C}" name="Status" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{6CEE09D4-5D6F-4E0A-9BE9-AE0EC38CA0B1}" name="Name" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{E3832498-CFA4-411F-8E36-3DCB0C21FD12}" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -790,6 +871,17 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E4BD95E9-018A-4366-A76C-4508FE6FBED8}" name="Table1" displayName="Table1" ref="C25:D28" totalsRowShown="0" tableBorderDxfId="5">
+  <autoFilter ref="C25:D28" xr:uid="{18B28362-03F1-4884-88EC-2590E82036F6}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{286918B6-6545-4A2F-AE22-A0117C86E89D}" name="Flying Mode"/>
+    <tableColumn id="2" xr3:uid="{BFD9BBEF-D0EC-4264-8FA9-1AE475A1F1B2}" name="Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{799FC318-1E9F-436A-9C85-84B4D29C8FE8}" name="Table5" displayName="Table5" ref="B10:D16" totalsRowShown="0">
   <autoFilter ref="B10:D16" xr:uid="{BA5FDCD0-D849-4F93-A4B1-5AEE8E3BE0A9}"/>
   <tableColumns count="3">
@@ -801,7 +893,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F4AFEA34-6A79-4FC1-A66C-4B694FE8402C}" name="Table6" displayName="Table6" ref="G10:I13" totalsRowShown="0" tableBorderDxfId="2">
   <autoFilter ref="G10:I13" xr:uid="{94B23AF5-C66B-46E7-BA0A-31D1EA2A2487}"/>
   <tableColumns count="3">
@@ -1132,11 +1224,11 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -1375,24 +1467,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF6C666-9F25-49C7-9F3E-23A20F280527}">
-  <dimension ref="B9:D22"/>
+  <dimension ref="B9:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="74.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -1443,10 +1537,10 @@
         <v>3</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
@@ -1454,10 +1548,10 @@
         <v>4</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
@@ -1465,10 +1559,10 @@
         <v>5</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -1476,47 +1570,73 @@
         <v>6</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="1">
-        <v>7</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" t="s">
-        <v>50</v>
-      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="3"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="1">
-        <v>8</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" t="s">
-        <v>66</v>
-      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="3"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D22" s="4" t="s">
         <v>80</v>
       </c>
     </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C24" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="15"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C27" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B9:D9"/>
+    <mergeCell ref="C24:D24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1526,7 +1646,7 @@
   <dimension ref="B9:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1542,16 +1662,16 @@
   </cols>
   <sheetData>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="G9" s="10" t="s">
+      <c r="C9" s="14"/>
+      <c r="D9" s="15"/>
+      <c r="G9" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="H9" s="11"/>
-      <c r="I9" s="12"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="18"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">

</xml_diff>

<commit_message>
2.7 Fixed Button constraints
</commit_message>
<xml_diff>
--- a/Drone Manual.xlsx
+++ b/Drone Manual.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoel1\Documents\Yoel\FIU\APAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83015882-398E-41FD-8ED1-F6B36DA09671}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC51F8F-5A37-4054-9432-1D52E99873AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DD67ECB3-E821-4B91-81DE-64EE5DC6E604}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{DD67ECB3-E821-4B91-81DE-64EE5DC6E604}"/>
   </bookViews>
   <sheets>
     <sheet name="Button Layout" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="115">
   <si>
     <t>Drone GUI</t>
   </si>
@@ -375,6 +375,12 @@
   </si>
   <si>
     <t xml:space="preserve">Manual for project version = </t>
+  </si>
+  <si>
+    <t>Navigation Comms</t>
+  </si>
+  <si>
+    <t>Video Comms</t>
   </si>
 </sst>
 </file>
@@ -591,7 +597,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -617,6 +623,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -624,6 +637,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
@@ -635,20 +657,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -666,17 +675,17 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -911,15 +920,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>322235</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>55535</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>426748</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>112727</xdr:rowOff>
+      <xdr:colOff>160048</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>150827</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -942,8 +951,57 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8770910" y="695325"/>
+          <a:off x="8504210" y="542925"/>
           <a:ext cx="6810113" cy="5703902"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>316123</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>107813</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>160914</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83F4FBB3-CB5B-42F6-AC55-D1DD42C65915}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11250823" y="1631813"/>
+          <a:ext cx="5256002" cy="3482101"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -994,8 +1052,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0C78C7B6-FE97-4068-A814-22972B595BD9}" name="Table4" displayName="Table4" ref="C5:E15" totalsRowShown="0">
   <autoFilter ref="C5:E15" xr:uid="{ECEF9464-F83C-46B5-8DD1-BC1CDD377798}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{659A9066-7A96-40CE-B5FB-AF590C26B6A5}" name="Code" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{E1B3786E-6997-4F8D-BE4F-7822846EAE70}" name="Name" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{659A9066-7A96-40CE-B5FB-AF590C26B6A5}" name="Code" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{E1B3786E-6997-4F8D-BE4F-7822846EAE70}" name="Name" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{BB63FDD6-5F93-4FD6-B09F-0D3EBEF4B562}" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1006,8 +1064,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{799FC318-1E9F-436A-9C85-84B4D29C8FE8}" name="Table5" displayName="Table5" ref="B10:D16" totalsRowShown="0">
   <autoFilter ref="B10:D16" xr:uid="{BA5FDCD0-D849-4F93-A4B1-5AEE8E3BE0A9}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{A1AB9263-4A07-43D7-A905-C26044E1CA27}" name="Position" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{EB512FA8-A3C2-4F60-96DA-9B891320BC11}" name="Name" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{A1AB9263-4A07-43D7-A905-C26044E1CA27}" name="Position" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{EB512FA8-A3C2-4F60-96DA-9B891320BC11}" name="Name" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{B05975E1-7AF0-4E77-8D4F-946199596813}" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1015,11 +1073,11 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F4AFEA34-6A79-4FC1-A66C-4B694FE8402C}" name="Table6" displayName="Table6" ref="G10:I13" totalsRowShown="0" tableBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F4AFEA34-6A79-4FC1-A66C-4B694FE8402C}" name="Table6" displayName="Table6" ref="G10:I13" totalsRowShown="0" tableBorderDxfId="2">
   <autoFilter ref="G10:I13" xr:uid="{94B23AF5-C66B-46E7-BA0A-31D1EA2A2487}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0AC0CAB2-4DC2-49CC-86E4-EC94125DA6F4}" name="Position" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{783BB960-6BC1-422A-A60D-A174EC46EDD5}" name="Name" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{0AC0CAB2-4DC2-49CC-86E4-EC94125DA6F4}" name="Position" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{783BB960-6BC1-422A-A60D-A174EC46EDD5}" name="Name" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{F2FEAD27-988A-4084-A5AD-E2555736FC1F}" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1325,8 +1383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5646660D-1CC2-4EB2-9448-3F3EBEA3AFF9}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1345,19 +1403,19 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="15">
         <v>2.7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="15"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="18"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -1610,7 +1668,7 @@
   <dimension ref="B9:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1622,11 +1680,11 @@
   </cols>
   <sheetData>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="18"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -1723,10 +1781,10 @@
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="D24" s="15"/>
+      <c r="D24" s="18"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
@@ -1925,7 +1983,7 @@
       </c>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="22" t="s">
+      <c r="E18" s="13" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1943,10 +2001,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B2ACA6E-8676-4667-B223-DF89C06D3E5D}">
-  <dimension ref="B9:I21"/>
+  <dimension ref="B7:S21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1962,19 +2020,42 @@
     <col min="13" max="13" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="13" t="s">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B7" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="K7" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="25"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15"/>
-      <c r="G9" s="16" t="s">
+      <c r="C9" s="17"/>
+      <c r="D9" s="18"/>
+      <c r="G9" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="18"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H9" s="23"/>
+      <c r="I9" s="24"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>31</v>
       </c>
@@ -1994,7 +2075,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>0</v>
       </c>
@@ -2014,7 +2095,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>1</v>
       </c>
@@ -2034,7 +2115,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>2</v>
       </c>
@@ -2054,7 +2135,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>3</v>
       </c>
@@ -2065,7 +2146,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>4</v>
       </c>
@@ -2076,7 +2157,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
@@ -2085,14 +2166,17 @@
       <c r="H21" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="G9:I9"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="K7:S7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>